<commit_message>
fix add new payment (remove middlware)
</commit_message>
<xml_diff>
--- a/תשלומים לקליטה 10.10.22.xlsx
+++ b/תשלומים לקליטה 10.10.22.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\VUE\Project-Payments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183ED16E-B341-4317-8A50-D044B3ACC9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C8C94F-BC0C-4766-9D12-1ABF1D096FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70EEBC19-9012-4D04-96C2-D989C0A19290}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{70EEBC19-9012-4D04-96C2-D989C0A19290}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$179</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$187</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="109">
   <si>
     <t>date</t>
   </si>
@@ -352,6 +352,18 @@
   </si>
   <si>
     <t>הוצאות אייל</t>
+  </si>
+  <si>
+    <t>אייל</t>
+  </si>
+  <si>
+    <t>לחמיס עבור נווה אליעזר</t>
+  </si>
+  <si>
+    <t>תומר -  13,200</t>
+  </si>
+  <si>
+    <t>תשלום עבור איטום + בטון רזה</t>
   </si>
 </sst>
 </file>
@@ -661,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -827,12 +839,59 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="86">
+  <dxfs count="88">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -2003,10 +2062,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C247C2-487C-40E1-BBBD-897A894D21CF}">
-  <dimension ref="A1:J179"/>
+  <dimension ref="A1:J187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D189" sqref="D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,7 +2074,7 @@
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -5782,7 +5842,7 @@
         <v>25000</v>
       </c>
       <c r="E132" s="3">
-        <f t="shared" ref="E132:E170" si="2">D132*0.17</f>
+        <f t="shared" ref="E132:E178" si="2">D132*0.17</f>
         <v>4250</v>
       </c>
       <c r="F132" s="3">
@@ -6779,7 +6839,9 @@
       <c r="A165" s="14">
         <v>44833</v>
       </c>
-      <c r="B165" s="1"/>
+      <c r="B165" s="1">
+        <v>3076</v>
+      </c>
       <c r="C165" s="2" t="s">
         <v>94</v>
       </c>
@@ -6802,25 +6864,27 @@
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A166" s="14">
+      <c r="A166" s="75">
         <v>44833</v>
       </c>
-      <c r="B166" s="1"/>
-      <c r="C166" s="2" t="s">
+      <c r="B166" s="76">
+        <v>3076</v>
+      </c>
+      <c r="C166" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="D166" s="3">
+      <c r="D166" s="78">
         <v>8000</v>
       </c>
-      <c r="E166" s="3">
+      <c r="E166" s="78">
         <f t="shared" si="2"/>
         <v>1360</v>
       </c>
-      <c r="F166" s="3">
+      <c r="F166" s="78">
         <f t="shared" si="9"/>
         <v>9360</v>
       </c>
-      <c r="G166" s="5">
+      <c r="G166" s="79">
         <v>10523</v>
       </c>
       <c r="J166" t="s">
@@ -6831,22 +6895,24 @@
       <c r="A167" s="14">
         <v>44833</v>
       </c>
-      <c r="B167" s="5"/>
-      <c r="C167" s="2" t="s">
+      <c r="B167" s="79">
+        <v>3076</v>
+      </c>
+      <c r="C167" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="D167" s="3">
+      <c r="D167" s="78">
         <v>8000</v>
       </c>
-      <c r="E167" s="3">
+      <c r="E167" s="78">
         <f t="shared" si="2"/>
         <v>1360</v>
       </c>
-      <c r="F167" s="3">
+      <c r="F167" s="78">
         <f t="shared" si="9"/>
         <v>9360</v>
       </c>
-      <c r="G167" s="5">
+      <c r="G167" s="79">
         <v>10523</v>
       </c>
       <c r="I167" t="s">
@@ -6860,22 +6926,24 @@
       <c r="A168" s="14">
         <v>44833</v>
       </c>
-      <c r="B168" s="5"/>
-      <c r="C168" s="2" t="s">
+      <c r="B168" s="82">
+        <v>3076</v>
+      </c>
+      <c r="C168" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D168" s="3">
+      <c r="D168" s="84">
         <v>1500</v>
       </c>
-      <c r="E168" s="3">
+      <c r="E168" s="84">
         <f t="shared" si="2"/>
         <v>255.00000000000003</v>
       </c>
-      <c r="F168" s="3">
+      <c r="F168" s="84">
         <f t="shared" si="9"/>
         <v>1755</v>
       </c>
-      <c r="G168" s="5">
+      <c r="G168" s="82">
         <v>10523</v>
       </c>
       <c r="I168" t="s">
@@ -6885,707 +6953,1028 @@
         <v>76</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="14">
         <v>44810</v>
       </c>
-      <c r="B169" s="37"/>
-      <c r="C169" s="70" t="s">
+      <c r="B169" s="85">
+        <v>3077</v>
+      </c>
+      <c r="C169" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="D169" s="36">
+      <c r="D169" s="86">
         <v>27000</v>
       </c>
-      <c r="E169" s="36">
+      <c r="E169" s="86">
         <f t="shared" si="2"/>
         <v>4590</v>
       </c>
-      <c r="F169" s="36">
+      <c r="F169" s="86">
         <f t="shared" si="9"/>
         <v>31590</v>
       </c>
-      <c r="G169" s="37">
+      <c r="G169" s="85">
         <v>10531</v>
       </c>
-      <c r="H169" s="39"/>
-      <c r="I169" s="39"/>
-      <c r="J169" s="39" t="s">
+      <c r="H169" s="81"/>
+      <c r="I169" s="81"/>
+      <c r="J169" s="81" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="14">
+        <v>44847</v>
+      </c>
+      <c r="B170" s="85">
+        <v>3081</v>
+      </c>
+      <c r="C170" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="D170" s="86">
+        <v>20000</v>
+      </c>
+      <c r="E170" s="86">
+        <f t="shared" si="2"/>
+        <v>3400.0000000000005</v>
+      </c>
+      <c r="F170" s="86">
+        <f t="shared" ref="F170:F177" si="10">SUM(D170:E170)</f>
+        <v>23400</v>
+      </c>
+      <c r="G170" s="85">
+        <v>10540</v>
+      </c>
+      <c r="H170" s="81"/>
+      <c r="I170" s="81"/>
+      <c r="J170" s="81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44853</v>
+      </c>
+      <c r="B171" s="85">
+        <v>3083</v>
+      </c>
+      <c r="C171" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="D171" s="86">
+        <v>20000</v>
+      </c>
+      <c r="E171" s="86">
+        <f t="shared" si="2"/>
+        <v>3400.0000000000005</v>
+      </c>
+      <c r="F171" s="86">
+        <f t="shared" si="10"/>
+        <v>23400</v>
+      </c>
+      <c r="G171" s="85">
+        <v>10542</v>
+      </c>
+      <c r="H171" s="81"/>
+      <c r="I171" s="81"/>
+      <c r="J171" s="81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44853</v>
+      </c>
+      <c r="B172" s="85">
+        <v>3083</v>
+      </c>
+      <c r="C172" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="D172" s="86">
+        <v>20000</v>
+      </c>
+      <c r="E172" s="86">
+        <f t="shared" si="2"/>
+        <v>3400.0000000000005</v>
+      </c>
+      <c r="F172" s="86">
+        <f t="shared" si="10"/>
+        <v>23400</v>
+      </c>
+      <c r="G172" s="85">
+        <v>10542</v>
+      </c>
+      <c r="H172" s="81"/>
+      <c r="I172" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="J172" s="81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44861</v>
+      </c>
+      <c r="B173" s="85">
+        <v>3084</v>
+      </c>
+      <c r="C173" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="D173" s="86">
+        <v>10000</v>
+      </c>
+      <c r="E173" s="86">
+        <f t="shared" si="2"/>
+        <v>1700.0000000000002</v>
+      </c>
+      <c r="F173" s="86">
+        <f t="shared" ref="F173" si="11">SUM(D173:E173)</f>
+        <v>11700</v>
+      </c>
+      <c r="G173" s="85">
+        <v>10550</v>
+      </c>
+      <c r="H173" s="81"/>
+      <c r="I173" s="81"/>
+      <c r="J173" s="81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44867</v>
+      </c>
+      <c r="B174" s="85">
+        <v>2132</v>
+      </c>
+      <c r="C174" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="D174" s="86">
+        <f>12000+13200</f>
+        <v>25200</v>
+      </c>
+      <c r="E174" s="86">
+        <f t="shared" si="2"/>
+        <v>4284</v>
+      </c>
+      <c r="F174" s="86">
+        <f t="shared" ref="F174" si="12">SUM(D174:E174)</f>
+        <v>29484</v>
+      </c>
+      <c r="G174" s="85">
+        <v>10555</v>
+      </c>
+      <c r="H174" s="81"/>
+      <c r="I174" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="J174" s="81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44875</v>
+      </c>
+      <c r="B175" s="85"/>
+      <c r="C175" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="D175" s="86">
+        <v>20000</v>
+      </c>
+      <c r="E175" s="86">
+        <f t="shared" si="2"/>
+        <v>3400.0000000000005</v>
+      </c>
+      <c r="F175" s="86">
+        <f t="shared" ref="F175:F177" si="13">SUM(D175:E175)</f>
+        <v>23400</v>
+      </c>
+      <c r="G175" s="85">
+        <v>10561</v>
+      </c>
+      <c r="H175" s="81"/>
+      <c r="I175" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="J175" s="81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44875</v>
+      </c>
+      <c r="B176" s="85"/>
+      <c r="C176" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="D176" s="86">
+        <v>9000</v>
+      </c>
+      <c r="E176" s="86">
+        <f t="shared" si="2"/>
+        <v>1530</v>
+      </c>
+      <c r="F176" s="86">
+        <f t="shared" si="13"/>
+        <v>10530</v>
+      </c>
+      <c r="G176" s="85">
+        <v>10561</v>
+      </c>
+      <c r="H176" s="81"/>
+      <c r="I176" s="81"/>
+      <c r="J176" s="81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="14">
+        <v>44875</v>
+      </c>
+      <c r="B177" s="33"/>
+      <c r="C177" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D177" s="35">
+        <v>1300</v>
+      </c>
+      <c r="E177" s="35">
+        <f t="shared" si="2"/>
+        <v>221.00000000000003</v>
+      </c>
+      <c r="F177" s="35">
+        <f t="shared" si="13"/>
+        <v>1521</v>
+      </c>
+      <c r="G177" s="33">
+        <v>10561</v>
+      </c>
+      <c r="H177" s="39"/>
+      <c r="I177" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="J177" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
         <v>44640</v>
       </c>
-      <c r="B170" s="1">
+      <c r="B178" s="1">
         <v>15</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="C178" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D170" s="3">
+      <c r="D178" s="3">
         <v>36500</v>
       </c>
-      <c r="E170" s="3">
+      <c r="E178" s="3">
         <f t="shared" si="2"/>
         <v>6205</v>
       </c>
-      <c r="F170" s="3">
-        <f>SUM(D170:E170)</f>
+      <c r="F178" s="3">
+        <f>SUM(D178:E178)</f>
         <v>42705</v>
       </c>
-      <c r="G170" s="5">
+      <c r="G178" s="5">
         <v>10387</v>
       </c>
-      <c r="H170">
+      <c r="H178">
         <v>5</v>
       </c>
-      <c r="J170" s="57" t="s">
+      <c r="J178" s="57" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A171" s="14">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="14">
         <v>44654</v>
       </c>
-      <c r="B171" s="5">
+      <c r="B179" s="5">
         <v>16</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C179" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D171" s="3">
+      <c r="D179" s="3">
         <v>16000</v>
       </c>
-      <c r="E171" s="3">
+      <c r="E179" s="3">
         <v>2720</v>
       </c>
-      <c r="F171" s="3">
+      <c r="F179" s="3">
         <v>18720</v>
       </c>
-      <c r="G171" s="5">
+      <c r="G179" s="5">
         <v>10399</v>
       </c>
-      <c r="H171">
+      <c r="H179">
         <v>5</v>
       </c>
-      <c r="J171" s="57" t="s">
+      <c r="J179" s="57" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A172" s="14">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
         <v>44679</v>
       </c>
-      <c r="B172" s="5">
+      <c r="B180" s="5">
         <v>18</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C180" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D172" s="3">
+      <c r="D180" s="3">
         <v>10000</v>
       </c>
-      <c r="E172" s="3">
+      <c r="E180" s="3">
         <v>1700.0000000000002</v>
       </c>
-      <c r="F172" s="3">
+      <c r="F180" s="3">
         <v>11700</v>
       </c>
-      <c r="G172" s="5">
+      <c r="G180" s="5">
         <v>10415</v>
       </c>
-      <c r="H172">
+      <c r="H180">
         <v>5</v>
       </c>
-      <c r="J172" s="57" t="s">
+      <c r="J180" s="57" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A173" s="14">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
         <v>44813</v>
       </c>
-      <c r="B173" s="1">
+      <c r="B181" s="1">
         <v>25</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C181" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D173" s="3">
+      <c r="D181" s="3">
         <v>75000</v>
       </c>
-      <c r="E173" s="3">
-        <f t="shared" ref="E173:E176" si="10">D173*0.17</f>
+      <c r="E181" s="3">
+        <f t="shared" ref="E181:E187" si="14">D181*0.17</f>
         <v>12750.000000000002</v>
       </c>
-      <c r="F173" s="3">
-        <f t="shared" ref="F173:F175" si="11">SUM(D173:E173)</f>
+      <c r="F181" s="3">
+        <f t="shared" ref="F181:F183" si="15">SUM(D181:E181)</f>
         <v>87750</v>
       </c>
-      <c r="G173" s="13" t="s">
+      <c r="G181" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="H173">
+      <c r="H181">
         <v>5</v>
       </c>
-      <c r="J173" s="57" t="s">
+      <c r="J181" s="57" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A174" s="14">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
         <v>44824</v>
       </c>
-      <c r="B174" s="1"/>
-      <c r="C174" s="2" t="s">
+      <c r="B182" s="88"/>
+      <c r="C182" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D174" s="4">
-        <f>F174/1.17</f>
+      <c r="D182" s="89">
+        <f>F182/1.17</f>
         <v>10256.410256410258</v>
       </c>
-      <c r="E174" s="4">
-        <f t="shared" si="10"/>
+      <c r="E182" s="89">
+        <f t="shared" si="14"/>
         <v>1743.5897435897439</v>
       </c>
-      <c r="F174" s="3">
+      <c r="F182" s="80">
         <v>12000</v>
       </c>
-      <c r="G174" s="3" t="s">
+      <c r="G182" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="H174" t="s">
+      <c r="H182" t="s">
         <v>63</v>
       </c>
-      <c r="J174" s="57" t="s">
+      <c r="J182" s="57" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="14">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
         <v>44825</v>
       </c>
-      <c r="B175" s="69">
+      <c r="B183" s="1">
         <v>27</v>
       </c>
-      <c r="C175" s="70" t="s">
+      <c r="C183" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D175" s="36">
+      <c r="D183" s="3">
         <v>59250</v>
       </c>
-      <c r="E175" s="36">
-        <f t="shared" si="10"/>
+      <c r="E183" s="3">
+        <f t="shared" si="14"/>
         <v>10072.5</v>
       </c>
-      <c r="F175" s="36">
-        <f t="shared" si="11"/>
+      <c r="F183" s="3">
+        <f t="shared" si="15"/>
         <v>69322.5</v>
       </c>
-      <c r="G175" s="36" t="s">
+      <c r="G183" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H175" s="39">
+      <c r="H183" s="2">
         <v>5</v>
       </c>
-      <c r="I175" s="39" t="s">
+      <c r="I183" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="J175" s="75" t="s">
+      <c r="J183" s="77" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A176" s="14">
-        <v>44640</v>
-      </c>
-      <c r="B176" s="1">
-        <v>15</v>
-      </c>
-      <c r="C176" s="2" t="s">
+    <row r="184" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="14">
+        <v>44867</v>
+      </c>
+      <c r="B184" s="69">
+        <v>29</v>
+      </c>
+      <c r="C184" s="70" t="s">
+        <v>78</v>
+      </c>
+      <c r="D184" s="36">
+        <v>55000</v>
+      </c>
+      <c r="E184" s="36">
+        <f t="shared" si="14"/>
+        <v>9350</v>
+      </c>
+      <c r="F184" s="36">
+        <f t="shared" ref="F184" si="16">SUM(D184:E184)</f>
+        <v>64350</v>
+      </c>
+      <c r="G184" s="37">
+        <v>10553</v>
+      </c>
+      <c r="H184" s="90">
+        <v>5</v>
+      </c>
+      <c r="I184" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="J184" s="90" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44712</v>
+      </c>
+      <c r="B185" s="1">
+        <v>113</v>
+      </c>
+      <c r="C185" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D176" s="3"/>
-      <c r="E176" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F176" s="3">
-        <f>SUM(D176:E176)</f>
-        <v>0</v>
-      </c>
-      <c r="G176" s="5">
-        <v>10387</v>
-      </c>
-      <c r="J176" t="s">
+      <c r="D185" s="3">
+        <v>10000</v>
+      </c>
+      <c r="E185" s="3">
+        <f t="shared" si="14"/>
+        <v>1700.0000000000002</v>
+      </c>
+      <c r="F185" s="3">
+        <f>SUM(D185:E185)</f>
+        <v>11700</v>
+      </c>
+      <c r="G185" s="5">
+        <v>10425</v>
+      </c>
+      <c r="H185">
+        <v>3</v>
+      </c>
+      <c r="J185" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A177" s="14">
-        <v>44654</v>
-      </c>
-      <c r="B177" s="5">
-        <v>16</v>
-      </c>
-      <c r="C177" s="2" t="s">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44857</v>
+      </c>
+      <c r="B186" s="5">
+        <v>118</v>
+      </c>
+      <c r="C186" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D177" s="3"/>
-      <c r="E177" s="3"/>
-      <c r="F177" s="3"/>
-      <c r="G177" s="5">
-        <v>10399</v>
-      </c>
-      <c r="J177" t="s">
+      <c r="D186" s="3">
+        <v>50000</v>
+      </c>
+      <c r="E186" s="3">
+        <f t="shared" si="14"/>
+        <v>8500</v>
+      </c>
+      <c r="F186" s="3">
+        <f t="shared" ref="F186:F187" si="17">SUM(D186:E186)</f>
+        <v>58500</v>
+      </c>
+      <c r="G186" s="5">
+        <v>10498</v>
+      </c>
+      <c r="H186">
+        <v>3</v>
+      </c>
+      <c r="J186" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A178" s="14">
-        <v>44679</v>
-      </c>
-      <c r="B178" s="5">
-        <v>18</v>
-      </c>
-      <c r="C178" s="2" t="s">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44857</v>
+      </c>
+      <c r="B187" s="5">
+        <v>119</v>
+      </c>
+      <c r="C187" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D178" s="3"/>
-      <c r="E178" s="3"/>
-      <c r="F178" s="3"/>
-      <c r="G178" s="5">
-        <v>10415</v>
-      </c>
-      <c r="J178" t="s">
+      <c r="D187" s="3">
+        <v>15000</v>
+      </c>
+      <c r="E187" s="3">
+        <f t="shared" si="14"/>
+        <v>2550</v>
+      </c>
+      <c r="F187" s="3">
+        <f t="shared" si="17"/>
+        <v>17550</v>
+      </c>
+      <c r="G187" s="5">
+        <v>10544</v>
+      </c>
+      <c r="H187">
+        <v>3</v>
+      </c>
+      <c r="J187" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="14">
-        <v>44813</v>
-      </c>
-      <c r="B179" s="69">
-        <v>25</v>
-      </c>
-      <c r="C179" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="D179" s="36">
-        <v>75000</v>
-      </c>
-      <c r="E179" s="36">
-        <f t="shared" ref="E179" si="12">D179*0.17</f>
-        <v>12750.000000000002</v>
-      </c>
-      <c r="F179" s="36">
-        <f t="shared" ref="F179" si="13">SUM(D179:E179)</f>
-        <v>87750</v>
-      </c>
-      <c r="G179" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="H179" s="39"/>
-      <c r="I179" s="39"/>
-      <c r="J179" s="39" t="s">
-        <v>102</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J179" xr:uid="{35C247C2-487C-40E1-BBBD-897A894D21CF}"/>
+  <autoFilter ref="A1:J187" xr:uid="{35C247C2-487C-40E1-BBBD-897A894D21CF}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G26 D2:D10 D13:D15 D17 D21:D23 E4:E27">
-    <cfRule type="cellIs" dxfId="85" priority="81" operator="equal">
+  <conditionalFormatting sqref="G26 D2:D10 D13:D15 D17 D21:D23 E4:E27 E166:E169 F160:F169">
+    <cfRule type="cellIs" dxfId="87" priority="98" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D12">
-    <cfRule type="cellIs" dxfId="84" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="97" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D27">
-    <cfRule type="cellIs" dxfId="83" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="96" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:F41 D43:F43">
-    <cfRule type="cellIs" dxfId="82" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="95" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42:F42">
-    <cfRule type="cellIs" dxfId="81" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="94" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:E44">
-    <cfRule type="cellIs" dxfId="80" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="93" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:F48">
-    <cfRule type="cellIs" dxfId="79" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="92" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:E49">
-    <cfRule type="cellIs" dxfId="78" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="91" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50:F52">
-    <cfRule type="cellIs" dxfId="77" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="90" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54:F54">
-    <cfRule type="cellIs" dxfId="76" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="89" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53:F53">
-    <cfRule type="cellIs" dxfId="75" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="88" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56:F56">
-    <cfRule type="cellIs" dxfId="74" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="87" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:F55">
-    <cfRule type="cellIs" dxfId="73" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="86" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:E57">
-    <cfRule type="cellIs" dxfId="72" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="85" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59:F59">
-    <cfRule type="cellIs" dxfId="71" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="84" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58:F58">
-    <cfRule type="cellIs" dxfId="70" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="83" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="69" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="82" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="cellIs" dxfId="68" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="81" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:F62">
-    <cfRule type="cellIs" dxfId="67" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="80" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61:F61">
-    <cfRule type="cellIs" dxfId="66" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="79" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:F64">
-    <cfRule type="cellIs" dxfId="65" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="78" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63:F63">
-    <cfRule type="cellIs" dxfId="64" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="77" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:F66 D68:F68">
-    <cfRule type="cellIs" dxfId="63" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="76" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:F65 D67:F67">
-    <cfRule type="cellIs" dxfId="62" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="75" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="cellIs" dxfId="61" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="74" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70:F70">
-    <cfRule type="cellIs" dxfId="60" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="73" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:F69">
-    <cfRule type="cellIs" dxfId="59" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="72" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71:E72">
-    <cfRule type="cellIs" dxfId="58" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="71" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71">
-    <cfRule type="cellIs" dxfId="57" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="70" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="56" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="69" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="55" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="68" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="54" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="53" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="52" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="65" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="51" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="50" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="63" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="49" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65 H67">
-    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="61" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69">
-    <cfRule type="cellIs" dxfId="47" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27:G31">
-    <cfRule type="cellIs" dxfId="46" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="59" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74:F77 D80:F80 D83:F88">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="57" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79:F79">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78:F78">
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81:F82">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92:E96">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91 D89:D91">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="53" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D130">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127:D128">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="51" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140:D142">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131:D139 E133:E142">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D152:E152 D154:E154">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E151 D149:D151">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F151:F152 F154">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D153">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G151">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G150">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D155">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F156:F157">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D156:D157">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G155:G157">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D158">
+    <cfRule type="cellIs" dxfId="25" priority="34" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E160:E165">
+    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G160">
+    <cfRule type="cellIs" dxfId="23" priority="30" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D181:E183">
+    <cfRule type="cellIs" dxfId="22" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F181:F183">
+    <cfRule type="cellIs" dxfId="21" priority="28" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D178:F178">
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D179:F179">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D180:F180">
+    <cfRule type="cellIs" dxfId="18" priority="25" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G181:G183">
+    <cfRule type="cellIs" dxfId="17" priority="24" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E170:E172">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E160:E165">
+  <conditionalFormatting sqref="F170:G171 F172">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E166:E169">
+  <conditionalFormatting sqref="E173">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F160:F169">
+  <conditionalFormatting sqref="F173:G173">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G160">
+  <conditionalFormatting sqref="E174">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D173:E175">
+  <conditionalFormatting sqref="F174:G174">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F173:F175">
+  <conditionalFormatting sqref="E175">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D170:F170">
+  <conditionalFormatting sqref="F175">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D171:F171">
+  <conditionalFormatting sqref="E176">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D172:F172">
+  <conditionalFormatting sqref="F176:G176">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G173:G175">
+  <conditionalFormatting sqref="E177">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D179:E179">
+  <conditionalFormatting sqref="F177:G177">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F179">
+  <conditionalFormatting sqref="D184:E184">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D176:F176">
+  <conditionalFormatting sqref="F184">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D177:F177">
+  <conditionalFormatting sqref="D185:F185 E186:F187">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D178:F178">
+  <conditionalFormatting sqref="D186">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G179">
+  <conditionalFormatting sqref="D187">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>